<commit_message>
actualizacion de prodcutos y categorias
</commit_message>
<xml_diff>
--- a/Comparativo bdWorkbench vs JAVA.xlsx
+++ b/Comparativo bdWorkbench vs JAVA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3efba4d0c9363e6c/cursos/DH/18 INTEGRADOR/Proyecto-Integrador-RopaDeDise-o/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3efba4d0c9363e6c/cursos/DH/00 cdsj/cdsj_integrador_02noviembre/Proyecto-Integrador-RopaDeDise-o/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="211" documentId="8_{41DE8B7F-ADCB-464E-9319-9EC43D5AE0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F068A139-8AA0-411F-8A12-FC453E2EC182}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{41DE8B7F-ADCB-464E-9319-9EC43D5AE0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB8B5F1A-4A3C-4E81-9989-76FC03E8E0F1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{690FC869-058A-473B-AA42-DB71106BD828}"/>
+    <workbookView minimized="1" xWindow="2460" yWindow="1485" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{690FC869-058A-473B-AA42-DB71106BD828}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLAS" sheetId="1" r:id="rId1"/>
@@ -438,13 +438,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>369809</xdr:colOff>
+      <xdr:colOff>760334</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>75190</xdr:rowOff>
     </xdr:to>
@@ -469,7 +469,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="390525" y="0"/>
           <a:ext cx="13323809" cy="8076190"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -850,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9CE717-EF69-4CDA-816C-630252591C88}">
   <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I40" sqref="I40"/>
     </sheetView>
@@ -1446,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19022DA2-EA9D-49E9-9058-569F46C9F7B3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>